<commit_message>
Added percentage growth from 2016-2017 and 2017-2018
</commit_message>
<xml_diff>
--- a/amazon_edit.xlsx
+++ b/amazon_edit.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://galvanizehq-my.sharepoint.com/personal/sean_reed_galvanizehq_onmicrosoft_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/excel/excel_work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{B59A292A-9934-4F49-8D4A-4DCF5B6A418E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE5AE362-FB7A-0745-843B-7ACE9F7BDE88}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4CFD18-821A-8043-80DE-DA7C0430B961}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15440" xr2:uid="{09650164-32A5-5E41-B315-3AC4BDEF06DC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16540" windowHeight="16260" xr2:uid="{09650164-32A5-5E41-B315-3AC4BDEF06DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Amazon-1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Total net sales</t>
   </si>
@@ -55,13 +56,37 @@
   </si>
   <si>
     <t>other expenses</t>
+  </si>
+  <si>
+    <t>Total Net Sales</t>
+  </si>
+  <si>
+    <t>Cost of Sales</t>
+  </si>
+  <si>
+    <t>Marketing Expenses</t>
+  </si>
+  <si>
+    <t>Other Expenses</t>
+  </si>
+  <si>
+    <t>Operating Income</t>
+  </si>
+  <si>
+    <t>2016- 2017 Percentage Growth</t>
+  </si>
+  <si>
+    <t>2017- 2018 Percentage Growth</t>
+  </si>
+  <si>
+    <t>Projections for 2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,16 +116,72 @@
       <color theme="1"/>
       <name val="Inherit"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB80001"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7B4FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -108,24 +189,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFB7B4FF"/>
+      <color rgb="FF9381FF"/>
+      <color rgb="FFB80001"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -437,7 +598,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A17"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -455,7 +616,7 @@
       <c r="B2" s="2">
         <v>2016</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="4"/>
       <c r="E2" s="2">
         <v>2017</v>
       </c>
@@ -464,241 +625,241 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="13">
         <v>135987</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="13">
         <v>177866</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="13">
         <v>232887</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="13">
         <v>88265</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="13">
         <v>111934</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="13">
         <v>139156</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="4"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="13">
         <v>7233</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="13">
         <v>10069</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="13">
         <v>13814</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="4"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="13">
         <f>B14-B8-B6</f>
         <v>36303</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="13">
         <f>E14-E8-E6</f>
         <v>51757</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5">
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="13">
         <f>H14-H8-H6</f>
         <v>67496</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="4"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="13">
         <v>131801</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5">
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="13">
         <v>173760</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="5">
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="13">
         <v>220466</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="4"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="13">
         <v>4186</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5">
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="13">
         <v>4106</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="5">
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="13">
         <v>12421</v>
       </c>
-      <c r="I16" s="4"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="4"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="3"/>
@@ -712,26 +873,26 @@
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="3"/>
@@ -745,26 +906,26 @@
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="4"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="4"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="3"/>
@@ -778,71 +939,82 @@
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="6"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="7"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="6"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="111">
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="K29:K30"/>
-    <mergeCell ref="L29:L30"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
+  <mergeCells count="55">
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:I22"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="H24:H25"/>
     <mergeCell ref="I24:I25"/>
@@ -859,88 +1031,153 @@
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="F24:F25"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5907B499-E589-944F-8AF7-352125E4A47D}">
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="21.83203125" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="27">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+      <c r="H1" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+    </row>
+    <row r="2" spans="1:14" ht="19">
+      <c r="A2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="12">
+        <f>('Amazon-1'!E3:E4-'Amazon-1'!B3:B4)/'Amazon-1'!B3:B4</f>
+        <v>0.30796326119408474</v>
+      </c>
+      <c r="B3" s="12">
+        <f>('Amazon-1'!E6-'Amazon-1'!B6)/'Amazon-1'!B6</f>
+        <v>0.26815838667648556</v>
+      </c>
+      <c r="C3" s="12">
+        <f>('Amazon-1'!E8-'Amazon-1'!B8)/'Amazon-1'!B8</f>
+        <v>0.39209180146550532</v>
+      </c>
+      <c r="D3" s="12">
+        <f>('Amazon-1'!E10-'Amazon-1'!B10)/'Amazon-1'!B10</f>
+        <v>0.42569484615596509</v>
+      </c>
+      <c r="E3" s="12">
+        <f>('Amazon-1'!E16-'Amazon-1'!B16)/'Amazon-1'!B16</f>
+        <v>-1.9111323459149548E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="27">
+      <c r="A7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" spans="1:14" ht="19">
+      <c r="A8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="12">
+        <f>('Amazon-1'!H3-'Amazon-1'!E3)/'Amazon-1'!E3</f>
+        <v>0.3093396152159491</v>
+      </c>
+      <c r="B9" s="12">
+        <f>('Amazon-1'!H6-'Amazon-1'!E6)/'Amazon-1'!E6</f>
+        <v>0.24319688387799954</v>
+      </c>
+      <c r="C9" s="12">
+        <f>('Amazon-1'!H8-'Amazon-1'!E8)/'Amazon-1'!E8</f>
+        <v>0.37193365776144605</v>
+      </c>
+      <c r="D9" s="12">
+        <f>('Amazon-1'!H10-'Amazon-1'!E10)/'Amazon-1'!E10</f>
+        <v>0.30409413219467896</v>
+      </c>
+      <c r="E9" s="12">
+        <f>('Amazon-1'!H16-'Amazon-1'!E16)/'Amazon-1'!E16</f>
+        <v>2.02508524111057</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added note with explanation of assumptions
</commit_message>
<xml_diff>
--- a/amazon_edit.xlsx
+++ b/amazon_edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/excel/excel_work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF200A1-9482-5643-8FAF-37B136989221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA981B4E-65EC-6145-991B-391C59E6122A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{09650164-32A5-5E41-B315-3AC4BDEF06DC}"/>
   </bookViews>
@@ -137,8 +137,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Galvanize</author>
+  </authors>
+  <commentList>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{BC321D9A-E94A-4B41-9233-A159575B5294}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Galvanize:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Total net sales</t>
   </si>
@@ -193,12 +227,16 @@
   <si>
     <t>Projections for 2019 and 2020</t>
   </si>
+  <si>
+    <t>For 2019-2020, I predict everything will continue on trend except for operating income, which I assume will spike a bit more.
+There was an article about Amazon not making as much profit in Q2 of 2019 because of rising transportation costs.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -261,6 +299,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -357,7 +408,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -402,7 +453,10 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5483,16 +5537,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>565150</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1479550</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1460500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5519,16 +5573,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>336550</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5555,16 +5609,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>882650</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5591,16 +5645,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>387350</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1301750</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5627,16 +5681,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>539750</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1454150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1441450</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5663,16 +5717,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>425450</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6459,11 +6513,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5907B499-E589-944F-8AF7-352125E4A47D}">
-  <dimension ref="A1:N9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5907B499-E589-944F-8AF7-352125E4A47D}">
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6559,14 +6613,10 @@
         <f>('Amazon-1'!E16-'Amazon-1'!B16)/'Amazon-1'!B16</f>
         <v>-1.9111323459149548E-2</v>
       </c>
-      <c r="G3" s="22">
-        <v>2019</v>
-      </c>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="1:14" ht="21">
-      <c r="G4" s="22">
-        <v>2020</v>
-      </c>
+      <c r="G4" s="22"/>
     </row>
     <row r="7" spans="1:14" ht="27">
       <c r="A7" s="16" t="s">
@@ -6616,8 +6666,14 @@
         <v>2.02508524111057</v>
       </c>
     </row>
+    <row r="13" spans="1:14" ht="221">
+      <c r="A13" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned up some extra text
</commit_message>
<xml_diff>
--- a/amazon_edit.xlsx
+++ b/amazon_edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/Documents/excel/excel_work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA981B4E-65EC-6145-991B-391C59E6122A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8CF456-7AA7-AC43-A3F2-20971A064B02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{09650164-32A5-5E41-B315-3AC4BDEF06DC}"/>
   </bookViews>
@@ -140,31 +140,18 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Galvanize</author>
+    <author>tc={33568108-B13E-0147-8DA7-F94F9BEC85AA}</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{BC321D9A-E94A-4B41-9233-A159575B5294}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{33568108-B13E-0147-8DA7-F94F9BEC85AA}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Galvanize:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    For 2019-2020, I predict everything will continue on trend except for operating income, which I assume will spike a bit more.
+There was an article about Amazon not making as much profit in Q2 of 2019 because of rising transportation costs.
+Reply:
+    I would also assume though Amazon said that this year was the highest selling Prime day ever, net sales will still continue to stay similar. Amazon Prime day in 2018 was the biggest ever before 2019, and the total net sales didn't grow</t>
       </text>
     </comment>
   </commentList>
@@ -172,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Total net sales</t>
   </si>
@@ -227,16 +214,12 @@
   <si>
     <t>Projections for 2019 and 2020</t>
   </si>
-  <si>
-    <t>For 2019-2020, I predict everything will continue on trend except for operating income, which I assume will spike a bit more.
-There was an article about Amazon not making as much profit in Q2 of 2019 because of rising transportation costs.</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -301,13 +284,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
@@ -5754,6 +5730,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Carlene Williams" id="{102CAF71-9983-594B-868E-226F7F9198C6}" userId="S::carlene.williams@galvanizehq.onmicrosoft.com::92d5ea84-26ec-4e4c-b559-f4d822deab63" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6047,6 +6029,18 @@
     </a:ext>
   </a:extLst>
 </a:theme>
+</file>
+
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H1" dT="2019-10-07T20:40:32.48" personId="{102CAF71-9983-594B-868E-226F7F9198C6}" id="{33568108-B13E-0147-8DA7-F94F9BEC85AA}">
+    <text>For 2019-2020, I predict everything will continue on trend except for operating income, which I assume will spike a bit more.
+There was an article about Amazon not making as much profit in Q2 of 2019 because of rising transportation costs.</text>
+  </threadedComment>
+  <threadedComment ref="H1" dT="2019-10-07T20:43:10.71" personId="{102CAF71-9983-594B-868E-226F7F9198C6}" id="{69AEA018-D3FC-C648-BCFA-DC9BA1240A23}" parentId="{33568108-B13E-0147-8DA7-F94F9BEC85AA}">
+    <text>I would also assume though Amazon said that this year was the highest selling Prime day ever, net sales will still continue to stay similar. Amazon Prime day in 2018 was the biggest ever before 2019, and the total net sales didn't grow</text>
+  </threadedComment>
+</ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6516,7 +6510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5907B499-E589-944F-8AF7-352125E4A47D}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -6666,10 +6660,8 @@
         <v>2.02508524111057</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="221">
-      <c r="A13" s="23" t="s">
-        <v>18</v>
-      </c>
+    <row r="13" spans="1:14">
+      <c r="A13" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>